<commit_message>
fund teorica conclupida versao final
</commit_message>
<xml_diff>
--- a/monografia v3/resultados (3).xlsx
+++ b/monografia v3/resultados (3).xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,33 +467,33 @@
       <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
+      <c r="B2">
+        <v>1180</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>1176</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3">
-        <f>B2/(B2+E2)</f>
-        <v>0.5</v>
+        <f t="shared" ref="F2:F12" si="0">B2/(B2+E2)</f>
+        <v>0.99830795262267347</v>
       </c>
       <c r="G2" s="3">
-        <f>C2/(C2+D2)</f>
-        <v>0.5</v>
+        <f t="shared" ref="G2:G12" si="1">C2/(C2+D2)</f>
+        <v>0.99408284023668636</v>
       </c>
       <c r="H2" s="3">
-        <f>(B2+C2)/(B2+C2+D2+E2)</f>
-        <v>0.5</v>
+        <f t="shared" ref="H2:H12" si="2">(B2+C2)/(B2+C2+D2+E2)</f>
+        <v>0.99619450317124736</v>
       </c>
       <c r="I2" s="3">
         <f>(D2+E2)/A16</f>
-        <v>7.776049766718507E-4</v>
+        <v>3.499222395023328E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -513,15 +513,15 @@
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <f>B3/(B3+E3)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G3" s="3">
-        <f>C3/(C3+D3)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H3" s="3">
-        <f>(B3+C3)/(B3+C3+D3+E3)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I3" s="3">
@@ -546,15 +546,15 @@
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <f>B4/(B4+E4)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G4" s="3">
-        <f>C4/(C4+D4)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H4" s="3">
-        <f>(B4+C4)/(B4+C4+D4+E4)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I4" s="3">
@@ -579,15 +579,15 @@
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <f>B5/(B5+E5)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G5" s="3">
-        <f>C5/(C5+D5)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H5" s="3">
-        <f>(B5+C5)/(B5+C5+D5+E5)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I5" s="3">
@@ -612,15 +612,15 @@
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <f>B6/(B6+E6)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G6" s="3">
-        <f>C6/(C6+D6)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H6" s="3">
-        <f>(B6+C6)/(B6+C6+D6+E6)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I6" s="3">
@@ -645,15 +645,15 @@
         <v>1</v>
       </c>
       <c r="F7" s="3">
-        <f>B7/(B7+E7)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G7" s="3">
-        <f>C7/(C7+D7)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H7" s="3">
-        <f>(B7+C7)/(B7+C7+D7+E7)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I7" s="3">
@@ -678,15 +678,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="3">
-        <f>B8/(B8+E8)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G8" s="3">
-        <f>C8/(C8+D8)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H8" s="3">
-        <f>(B8+C8)/(B8+C8+D8+E8)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I8" s="3">
@@ -711,15 +711,15 @@
         <v>1</v>
       </c>
       <c r="F9" s="3">
-        <f>B9/(B9+E9)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G9" s="3">
-        <f>C9/(C9+D9)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H9" s="3">
-        <f>(B9+C9)/(B9+C9+D9+E9)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I9" s="3">
@@ -744,15 +744,15 @@
         <v>1</v>
       </c>
       <c r="F10" s="3">
-        <f>B10/(B10+E10)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G10" s="3">
-        <f>C10/(C10+D10)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H10" s="3">
-        <f>(B10+C10)/(B10+C10+D10+E10)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I10" s="3">
@@ -777,15 +777,15 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <f>B11/(B11+E11)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G11" s="3">
-        <f>C11/(C11+D11)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H11" s="3">
-        <f>(B11+C11)/(B11+C11+D11+E11)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I11" s="3">
@@ -810,15 +810,15 @@
         <v>1</v>
       </c>
       <c r="F12" s="3">
-        <f>B12/(B12+E12)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G12" s="3">
-        <f>C12/(C12+D12)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="H12" s="3">
-        <f>(B12+C12)/(B12+C12+D12+E12)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I12" s="3">

</xml_diff>

<commit_message>
nova uml, resultados kohonen
</commit_message>
<xml_diff>
--- a/monografia v3/resultados (3).xlsx
+++ b/monografia v3/resultados (3).xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,32 +468,32 @@
         <v>0</v>
       </c>
       <c r="B2">
+        <v>1177</v>
+      </c>
+      <c r="C2">
         <v>1180</v>
       </c>
-      <c r="C2" s="3">
-        <v>1176</v>
-      </c>
-      <c r="D2" s="3">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F12" si="0">B2/(B2+E2)</f>
-        <v>0.99830795262267347</v>
+        <v>0.99576988155668356</v>
       </c>
       <c r="G2" s="3">
         <f t="shared" ref="G2:G12" si="1">C2/(C2+D2)</f>
-        <v>0.99408284023668636</v>
+        <v>0.99915325994919557</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ref="H2:H12" si="2">(B2+C2)/(B2+C2+D2+E2)</f>
-        <v>0.99619450317124736</v>
+        <v>0.99746085484553537</v>
       </c>
       <c r="I2" s="3">
         <f>(D2+E2)/A16</f>
-        <v>3.499222395023328E-3</v>
+        <v>2.3328149300155523E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -839,6 +839,9 @@
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
+      <c r="G16">
+        <v>1182</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">

</xml_diff>